<commit_message>
add new places and change githib link
</commit_message>
<xml_diff>
--- a/places.xlsx
+++ b/places.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andy\OneDrive - University College London\General\website\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53FD7E12-8381-49BA-9819-EF796E3FE353}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BB65477-C297-4507-B0C3-E2E69513D3A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13770" yWindow="2850" windowWidth="43200" windowHeight="12330" xr2:uid="{6362DE6B-9A95-49B5-8331-B8A2B0F11EDC}"/>
+    <workbookView xWindow="-75" yWindow="0" windowWidth="8790" windowHeight="10155" xr2:uid="{6362DE6B-9A95-49B5-8331-B8A2B0F11EDC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="36">
   <si>
     <t>Time</t>
   </si>
@@ -68,9 +68,6 @@
     <t xml:space="preserve">Tenerife </t>
   </si>
   <si>
-    <t xml:space="preserve">Cambodia </t>
-  </si>
-  <si>
     <t>UCL</t>
   </si>
   <si>
@@ -119,9 +116,6 @@
     <t>Dension barracks</t>
   </si>
   <si>
-    <t>Examiner</t>
-  </si>
-  <si>
     <t>University of Oxford</t>
   </si>
   <si>
@@ -138,6 +132,18 @@
   </si>
   <si>
     <t>Lecturer</t>
+  </si>
+  <si>
+    <t>Phnom Penh</t>
+  </si>
+  <si>
+    <t>Angkor Wat</t>
+  </si>
+  <si>
+    <t>External Examiner</t>
+  </si>
+  <si>
+    <t>Pretoria</t>
   </si>
 </sst>
 </file>
@@ -512,19 +518,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B245866-484B-4C42-BB5F-73A7295E0F38}">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="R13" sqref="R13"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="1" max="1" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -532,16 +538,16 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" t="s">
         <v>23</v>
       </c>
-      <c r="E1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -549,7 +555,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D2">
         <v>-34.424393999999999</v>
@@ -558,66 +564,66 @@
         <v>150.89384999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D3">
-        <v>-29.116395000000001</v>
+        <v>-25.745937000000001</v>
       </c>
       <c r="E3">
-        <v>26.215496000000002</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>28.187944000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="B4" t="s">
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D4">
+        <v>-29.116395000000001</v>
+      </c>
+      <c r="E4">
+        <v>26.215496000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5">
         <v>53.381504</v>
       </c>
-      <c r="E4">
+      <c r="E5">
         <v>-1.4833689999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5">
-        <v>50.961756999999999</v>
-      </c>
-      <c r="E5">
-        <v>-1.4239980000000001</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="D6">
         <v>50.961756999999999</v>
@@ -626,228 +632,263 @@
         <v>-1.4239980000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A7" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
         <v>3</v>
       </c>
       <c r="C7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7">
+        <v>50.961756999999999</v>
+      </c>
+      <c r="E7">
+        <v>-1.4239980000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A8" t="s">
         <v>21</v>
       </c>
-      <c r="D7">
+      <c r="B8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8">
         <v>48.208354</v>
       </c>
-      <c r="E7">
+      <c r="E8">
         <v>16.372503999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" t="s">
         <v>20</v>
       </c>
-      <c r="B8" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" t="s">
-        <v>21</v>
-      </c>
-      <c r="D8">
+      <c r="D9">
         <v>-34.928181000000002</v>
       </c>
-      <c r="E8">
+      <c r="E9">
         <v>138.599931</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A10" t="s">
         <v>4</v>
       </c>
-      <c r="B9" t="s">
-        <v>3</v>
-      </c>
-      <c r="C9" t="s">
-        <v>3</v>
-      </c>
-      <c r="D9">
+      <c r="B10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10">
         <v>-31.950403999999999</v>
       </c>
-      <c r="E9">
+      <c r="E10">
         <v>115.79790199999999</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A11" t="s">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
-        <v>3</v>
-      </c>
-      <c r="C10" t="s">
+      <c r="B11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11">
+        <v>28.293578</v>
+      </c>
+      <c r="E11">
+        <v>-16.621447</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A12" t="s">
         <v>17</v>
       </c>
-      <c r="D10">
-        <v>28.293578</v>
-      </c>
-      <c r="E10">
-        <v>-16.621447</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" t="s">
-        <v>3</v>
-      </c>
-      <c r="C11" t="s">
-        <v>17</v>
-      </c>
-      <c r="D11">
+      <c r="B12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12">
         <v>39.469901</v>
       </c>
-      <c r="E11">
+      <c r="E12">
         <v>-0.37595099999999998</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A13" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13">
+        <v>13.4125</v>
+      </c>
+      <c r="E13">
+        <v>103.866569</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A14" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14">
+        <v>11.568270999999999</v>
+      </c>
+      <c r="E14">
+        <v>104.922443</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="29.5" x14ac:dyDescent="0.75">
+      <c r="A15" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" t="s">
         <v>10</v>
       </c>
-      <c r="B12" t="s">
-        <v>3</v>
-      </c>
-      <c r="C12" t="s">
-        <v>17</v>
-      </c>
-      <c r="D12">
-        <v>13.506639</v>
-      </c>
-      <c r="E12">
-        <v>104.869423</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+      <c r="C15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15">
+        <v>17.592275000000001</v>
+      </c>
+      <c r="E15">
+        <v>78.122189000000006</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A16" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16">
+        <v>53.797418</v>
+      </c>
+      <c r="E16">
+        <v>-1.5437940000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A17" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" t="s">
+        <v>20</v>
+      </c>
+      <c r="D17">
+        <v>55.861154999999997</v>
+      </c>
+      <c r="E17">
+        <v>-4.2501689999999996</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A18" t="s">
         <v>25</v>
       </c>
-      <c r="B13" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" t="s">
-        <v>12</v>
-      </c>
-      <c r="D13">
-        <v>17.592275000000001</v>
-      </c>
-      <c r="E13">
-        <v>78.122189000000006</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="B18" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" t="s">
+        <v>34</v>
+      </c>
+      <c r="D18">
+        <v>51.454070999999999</v>
+      </c>
+      <c r="E18">
+        <v>-1.285677</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A19" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" t="s">
+        <v>29</v>
+      </c>
+      <c r="D19">
+        <v>51.758707999999999</v>
+      </c>
+      <c r="E19">
+        <v>-1.255668</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A20" t="s">
         <v>30</v>
       </c>
-      <c r="B14" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" t="s">
-        <v>21</v>
-      </c>
-      <c r="D14">
-        <v>53.797418</v>
-      </c>
-      <c r="E14">
-        <v>-1.5437940000000001</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>29</v>
-      </c>
-      <c r="B15" t="s">
-        <v>11</v>
-      </c>
-      <c r="C15" t="s">
-        <v>21</v>
-      </c>
-      <c r="D15">
-        <v>55.861154999999997</v>
-      </c>
-      <c r="E15">
-        <v>-4.2501689999999996</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>26</v>
-      </c>
-      <c r="B16" t="s">
-        <v>11</v>
-      </c>
-      <c r="C16" t="s">
-        <v>27</v>
-      </c>
-      <c r="D16">
-        <v>51.454070999999999</v>
-      </c>
-      <c r="E16">
-        <v>-1.285677</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>28</v>
-      </c>
-      <c r="B17" t="s">
-        <v>11</v>
-      </c>
-      <c r="C17" t="s">
+      <c r="B20" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" t="s">
         <v>31</v>
       </c>
-      <c r="D17">
-        <v>51.758707999999999</v>
-      </c>
-      <c r="E17">
-        <v>-1.255668</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>32</v>
-      </c>
-      <c r="B18" t="s">
-        <v>11</v>
-      </c>
-      <c r="C18" t="s">
-        <v>33</v>
-      </c>
-      <c r="D18">
+      <c r="D20">
         <v>51.507322000000002</v>
       </c>
-      <c r="E18">
+      <c r="E20">
         <v>-0.12764700000000001</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A21" t="s">
         <v>6</v>
       </c>
-      <c r="B19" t="s">
-        <v>11</v>
-      </c>
-      <c r="C19" t="s">
-        <v>21</v>
-      </c>
-      <c r="D19">
+      <c r="B21" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" t="s">
+        <v>20</v>
+      </c>
+      <c r="D21">
         <v>53.381504</v>
       </c>
-      <c r="E19">
+      <c r="E21">
         <v>-1.4833689999999999</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>